<commit_message>
small updates to phase shift analysis
need to revisit and refactor
</commit_message>
<xml_diff>
--- a/contact_correlations/phaseshift/phaseshift_summary.xlsx
+++ b/contact_correlations/phaseshift/phaseshift_summary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/phaseshift/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unobtainium\E_Carmen_Santiago\Analysis Scripts\analysis\contact_correlations\phaseshift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1D9C99-B8EF-FF4D-9201-3D996B82C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="735" windowWidth="28035" windowHeight="16875"/>
   </bookViews>
   <sheets>
     <sheet name="phaseshift_metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>filename</t>
   </si>
@@ -137,12 +136,21 @@
   </si>
   <si>
     <t>2024-06-18_D_e.dat</t>
+  </si>
+  <si>
+    <t>ps</t>
+  </si>
+  <si>
+    <t>e_ps</t>
+  </si>
+  <si>
+    <t>Amp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -977,19 +985,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1017,8 +1025,17 @@
       <c r="I1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1105,7 +1122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1134,7 +1151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1189,7 +1206,7 @@
         <v>202.1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1215,7 +1232,7 @@
         <v>202.1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1258,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1267,7 +1284,7 @@
         <v>202.14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1292,8 +1309,17 @@
       <c r="H11">
         <v>202</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K11">
+        <v>0.41</v>
+      </c>
+      <c r="L11">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1318,8 +1344,17 @@
       <c r="H12">
         <v>202</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.34</v>
+      </c>
+      <c r="K12">
+        <v>0.12</v>
+      </c>
+      <c r="L12">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1344,8 +1379,17 @@
       <c r="H13">
         <v>202</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0.17</v>
+      </c>
+      <c r="K13">
+        <v>0.27</v>
+      </c>
+      <c r="L13">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1370,8 +1414,17 @@
       <c r="H14">
         <v>202</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>0.22</v>
+      </c>
+      <c r="K14">
+        <v>0.15</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1396,8 +1449,17 @@
       <c r="H15">
         <v>202</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>0.33</v>
+      </c>
+      <c r="K15">
+        <v>0.17</v>
+      </c>
+      <c r="L15">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1422,8 +1484,17 @@
       <c r="H16">
         <v>202</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K16">
+        <v>0.2</v>
+      </c>
+      <c r="L16">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1448,8 +1519,17 @@
       <c r="H17">
         <v>202</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>0.27</v>
+      </c>
+      <c r="K17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L17">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1474,8 +1554,17 @@
       <c r="H18">
         <v>202</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>0.27</v>
+      </c>
+      <c r="K18">
+        <v>0.19</v>
+      </c>
+      <c r="L18">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1499,6 +1588,15 @@
       </c>
       <c r="H19">
         <v>202</v>
+      </c>
+      <c r="J19">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="K19">
+        <v>0.22</v>
+      </c>
+      <c r="L19">
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>